<commit_message>
More queries and contracts
</commit_message>
<xml_diff>
--- a/templates/precios.xlsx
+++ b/templates/precios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\Development\projects\ciber\cotown\back\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF108ED6-C229-4389-AAA3-7E3863B4D559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{261FE050-1BEB-4E5D-B407-A77EB1D88DCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -140,6 +140,7 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -195,11 +196,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="hair">
-        <color rgb="FFC6C6C6"/>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
       </left>
-      <right style="hair">
-        <color rgb="FFC6C6C6"/>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
       </right>
       <top/>
       <bottom/>
@@ -222,14 +223,14 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="15" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
@@ -633,14 +634,14 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="7"/>
+      <c r="E1" s="6"/>
       <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
@@ -710,22 +711,22 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
     </row>
     <row r="4" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>

</xml_diff>